<commit_message>
Poder utilizar diferentes Class en Reporte Excel
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOSHIBA\Dropbox\Proyecto SEC\Reportes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teto\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Modelo de Gestión por Competencias</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Tomar decisiones en el momento</t>
-  </si>
-  <si>
-    <t>Administrar el tiempo</t>
   </si>
   <si>
     <t>Candidato Ideal</t>
@@ -200,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -210,14 +207,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,8 +225,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -248,7 +257,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -316,7 +325,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-CR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1070,9 +1079,6 @@
               <c:f>Hoja1!$E$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Administrar el tiempo</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1131,9 +1137,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1148,11 +1151,11 @@
         </c:dLbls>
         <c:gapWidth val="355"/>
         <c:overlap val="-70"/>
-        <c:axId val="257144816"/>
-        <c:axId val="257145376"/>
+        <c:axId val="165985568"/>
+        <c:axId val="165985960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="257144816"/>
+        <c:axId val="165985568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1192,10 +1195,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257145376"/>
+        <c:crossAx val="165985960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1203,7 +1206,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="257145376"/>
+        <c:axId val="165985960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,7 +1289,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-MX"/>
+              <a:endParaRPr lang="es-CR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1318,10 +1321,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257144816"/>
+        <c:crossAx val="165985568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1361,7 +1364,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-CR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1391,7 +1394,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-CR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1405,7 +1408,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1468,7 +1471,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-CR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1534,7 +1537,7 @@
             <c:strRef>
               <c:f>Hoja1!$E$34:$E$44</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Capacitación Formal</c:v>
                 </c:pt>
@@ -1564,9 +1567,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Tomar decisiones en el momento</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Administrar el tiempo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1606,9 +1606,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1670,7 +1667,7 @@
             <c:strRef>
               <c:f>Hoja1!$E$34:$E$44</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Capacitación Formal</c:v>
                 </c:pt>
@@ -1700,9 +1697,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Tomar decisiones en el momento</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Administrar el tiempo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1725,11 +1719,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="257148736"/>
-        <c:axId val="257149296"/>
+        <c:axId val="166808368"/>
+        <c:axId val="166808760"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="257148736"/>
+        <c:axId val="166808368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1769,10 +1763,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257149296"/>
+        <c:crossAx val="166808760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1780,7 +1774,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="257149296"/>
+        <c:axId val="166808760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1828,10 +1822,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257148736"/>
+        <c:crossAx val="166808368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1871,7 +1865,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-CR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1901,7 +1895,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-CR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3157,7 +3151,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3421,11 +3415,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43:I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
@@ -3440,133 +3434,133 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="H4" s="10" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="H4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="H5" s="10" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="H5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="H6" s="10" t="s">
+      <c r="D6" s="8"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="H6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="H7" s="10" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="H7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="33" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="9"/>
+      <c r="F33" s="10"/>
       <c r="G33" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="34" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="8"/>
+      <c r="F34" s="9"/>
       <c r="G34" s="3">
         <v>2</v>
       </c>
@@ -3576,10 +3570,10 @@
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="8"/>
+      <c r="F35" s="9"/>
       <c r="G35" s="3">
         <v>2</v>
       </c>
@@ -3589,10 +3583,10 @@
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="8"/>
+      <c r="F36" s="9"/>
       <c r="G36" s="3">
         <v>3</v>
       </c>
@@ -3602,10 +3596,10 @@
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="8"/>
+      <c r="F37" s="9"/>
       <c r="G37" s="3">
         <v>4</v>
       </c>
@@ -3615,10 +3609,10 @@
       <c r="I37" s="4"/>
     </row>
     <row r="38" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F38" s="8"/>
+      <c r="F38" s="9"/>
       <c r="G38" s="3">
         <v>5</v>
       </c>
@@ -3628,10 +3622,10 @@
       <c r="I38" s="4"/>
     </row>
     <row r="39" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="8"/>
+      <c r="F39" s="9"/>
       <c r="G39" s="3">
         <v>6</v>
       </c>
@@ -3641,10 +3635,10 @@
       <c r="I39" s="4"/>
     </row>
     <row r="40" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F40" s="8"/>
+      <c r="F40" s="9"/>
       <c r="G40" s="3">
         <v>3</v>
       </c>
@@ -3654,10 +3648,10 @@
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="8"/>
+      <c r="F41" s="9"/>
       <c r="G41" s="3">
         <v>4</v>
       </c>
@@ -3667,10 +3661,10 @@
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F42" s="8"/>
+      <c r="F42" s="9"/>
       <c r="G42" s="3">
         <v>5</v>
       </c>
@@ -3680,11 +3674,11 @@
       <c r="I42" s="4"/>
     </row>
     <row r="43" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="8"/>
-      <c r="G43" s="3">
+      <c r="F43" s="9"/>
+      <c r="G43" s="5">
         <v>3</v>
       </c>
       <c r="H43" s="4">
@@ -3693,20 +3687,31 @@
       <c r="I43" s="4"/>
     </row>
     <row r="44" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E44" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="3">
-        <v>2</v>
-      </c>
-      <c r="H44" s="4">
-        <v>2</v>
-      </c>
-      <c r="I44" s="4"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="A10:L10"/>
@@ -3722,23 +3727,6 @@
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J7:K7"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="55" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Creacion de reporte EC
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOSHIBA\Dropbox\Proyecto SEC\Reportes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teto\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Modelo de Gestión por Competencias</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Tomar decisiones en el momento</t>
-  </si>
-  <si>
-    <t>Administrar el tiempo</t>
   </si>
   <si>
     <t>Candidato Ideal</t>
@@ -200,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -210,14 +207,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,8 +225,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -248,7 +257,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -316,7 +325,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-CR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1070,9 +1079,6 @@
               <c:f>Hoja1!$E$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Administrar el tiempo</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1131,9 +1137,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1148,11 +1151,11 @@
         </c:dLbls>
         <c:gapWidth val="355"/>
         <c:overlap val="-70"/>
-        <c:axId val="257144816"/>
-        <c:axId val="257145376"/>
+        <c:axId val="165985568"/>
+        <c:axId val="165985960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="257144816"/>
+        <c:axId val="165985568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1192,10 +1195,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257145376"/>
+        <c:crossAx val="165985960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1203,7 +1206,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="257145376"/>
+        <c:axId val="165985960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,7 +1289,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-MX"/>
+              <a:endParaRPr lang="es-CR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1318,10 +1321,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257144816"/>
+        <c:crossAx val="165985568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1361,7 +1364,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-CR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1391,7 +1394,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-CR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1405,7 +1408,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1468,7 +1471,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-CR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1534,7 +1537,7 @@
             <c:strRef>
               <c:f>Hoja1!$E$34:$E$44</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Capacitación Formal</c:v>
                 </c:pt>
@@ -1564,9 +1567,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Tomar decisiones en el momento</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Administrar el tiempo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1606,9 +1606,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1670,7 +1667,7 @@
             <c:strRef>
               <c:f>Hoja1!$E$34:$E$44</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Capacitación Formal</c:v>
                 </c:pt>
@@ -1700,9 +1697,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Tomar decisiones en el momento</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Administrar el tiempo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1725,11 +1719,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="257148736"/>
-        <c:axId val="257149296"/>
+        <c:axId val="166808368"/>
+        <c:axId val="166808760"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="257148736"/>
+        <c:axId val="166808368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1769,10 +1763,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257149296"/>
+        <c:crossAx val="166808760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1780,7 +1774,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="257149296"/>
+        <c:axId val="166808760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1828,10 +1822,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257148736"/>
+        <c:crossAx val="166808368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1871,7 +1865,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-CR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1901,7 +1895,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-CR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3157,7 +3151,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3421,11 +3415,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43:I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
@@ -3440,133 +3434,133 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="H4" s="10" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="H4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="H5" s="10" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="H5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="H6" s="10" t="s">
+      <c r="D6" s="8"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="H6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="H7" s="10" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="H7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="33" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="9"/>
+      <c r="F33" s="10"/>
       <c r="G33" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="34" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="8"/>
+      <c r="F34" s="9"/>
       <c r="G34" s="3">
         <v>2</v>
       </c>
@@ -3576,10 +3570,10 @@
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="8"/>
+      <c r="F35" s="9"/>
       <c r="G35" s="3">
         <v>2</v>
       </c>
@@ -3589,10 +3583,10 @@
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="8"/>
+      <c r="F36" s="9"/>
       <c r="G36" s="3">
         <v>3</v>
       </c>
@@ -3602,10 +3596,10 @@
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="8"/>
+      <c r="F37" s="9"/>
       <c r="G37" s="3">
         <v>4</v>
       </c>
@@ -3615,10 +3609,10 @@
       <c r="I37" s="4"/>
     </row>
     <row r="38" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F38" s="8"/>
+      <c r="F38" s="9"/>
       <c r="G38" s="3">
         <v>5</v>
       </c>
@@ -3628,10 +3622,10 @@
       <c r="I38" s="4"/>
     </row>
     <row r="39" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="8"/>
+      <c r="F39" s="9"/>
       <c r="G39" s="3">
         <v>6</v>
       </c>
@@ -3641,10 +3635,10 @@
       <c r="I39" s="4"/>
     </row>
     <row r="40" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F40" s="8"/>
+      <c r="F40" s="9"/>
       <c r="G40" s="3">
         <v>3</v>
       </c>
@@ -3654,10 +3648,10 @@
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="8"/>
+      <c r="F41" s="9"/>
       <c r="G41" s="3">
         <v>4</v>
       </c>
@@ -3667,10 +3661,10 @@
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F42" s="8"/>
+      <c r="F42" s="9"/>
       <c r="G42" s="3">
         <v>5</v>
       </c>
@@ -3680,11 +3674,11 @@
       <c r="I42" s="4"/>
     </row>
     <row r="43" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="8"/>
-      <c r="G43" s="3">
+      <c r="F43" s="9"/>
+      <c r="G43" s="5">
         <v>3</v>
       </c>
       <c r="H43" s="4">
@@ -3693,20 +3687,31 @@
       <c r="I43" s="4"/>
     </row>
     <row r="44" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E44" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="3">
-        <v>2</v>
-      </c>
-      <c r="H44" s="4">
-        <v>2</v>
-      </c>
-      <c r="I44" s="4"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="A10:L10"/>
@@ -3722,23 +3727,6 @@
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J7:K7"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="55" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Mostrar promedio ponderado, y nombre de meritos y competencias en el reporte
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Modelo de Gestión por Competencias</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Valor Relativo</t>
+  </si>
+  <si>
+    <t>Promedio ponderado</t>
   </si>
 </sst>
 </file>
@@ -197,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -210,6 +213,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -219,22 +234,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1151,11 +1157,11 @@
         </c:dLbls>
         <c:gapWidth val="355"/>
         <c:overlap val="-70"/>
-        <c:axId val="165985568"/>
-        <c:axId val="165985960"/>
+        <c:axId val="165174144"/>
+        <c:axId val="165153216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="165985568"/>
+        <c:axId val="165174144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1198,7 +1204,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165985960"/>
+        <c:crossAx val="165153216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1206,7 +1212,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165985960"/>
+        <c:axId val="165153216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1324,7 +1330,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165985568"/>
+        <c:crossAx val="165174144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1719,11 +1725,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166808368"/>
-        <c:axId val="166808760"/>
+        <c:axId val="164177552"/>
+        <c:axId val="164177944"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="166808368"/>
+        <c:axId val="164177552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1766,7 +1772,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166808760"/>
+        <c:crossAx val="164177944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1774,7 +1780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166808760"/>
+        <c:axId val="164177944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1825,7 +1831,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166808368"/>
+        <c:crossAx val="164177552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3413,10 +3419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43:I43"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46:F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3434,118 +3440,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="H4" s="8" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="H4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="H5" s="8" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="H5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="H6" s="8" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="H6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="H7" s="8" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="H7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="33" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="10"/>
+      <c r="F33" s="8"/>
       <c r="G33" s="2" t="s">
         <v>23</v>
       </c>
@@ -3557,10 +3563,10 @@
       </c>
     </row>
     <row r="34" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="9"/>
+      <c r="F34" s="14"/>
       <c r="G34" s="3">
         <v>2</v>
       </c>
@@ -3570,10 +3576,10 @@
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="9"/>
+      <c r="F35" s="14"/>
       <c r="G35" s="3">
         <v>2</v>
       </c>
@@ -3583,10 +3589,10 @@
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="9"/>
+      <c r="F36" s="14"/>
       <c r="G36" s="3">
         <v>3</v>
       </c>
@@ -3596,10 +3602,10 @@
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="9"/>
+      <c r="F37" s="14"/>
       <c r="G37" s="3">
         <v>4</v>
       </c>
@@ -3609,10 +3615,10 @@
       <c r="I37" s="4"/>
     </row>
     <row r="38" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E38" s="9" t="s">
+      <c r="E38" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F38" s="9"/>
+      <c r="F38" s="14"/>
       <c r="G38" s="3">
         <v>5</v>
       </c>
@@ -3622,10 +3628,10 @@
       <c r="I38" s="4"/>
     </row>
     <row r="39" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="9"/>
+      <c r="F39" s="14"/>
       <c r="G39" s="3">
         <v>6</v>
       </c>
@@ -3635,10 +3641,10 @@
       <c r="I39" s="4"/>
     </row>
     <row r="40" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F40" s="9"/>
+      <c r="F40" s="14"/>
       <c r="G40" s="3">
         <v>3</v>
       </c>
@@ -3648,10 +3654,10 @@
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="9"/>
+      <c r="F41" s="14"/>
       <c r="G41" s="3">
         <v>4</v>
       </c>
@@ -3661,10 +3667,10 @@
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E42" s="9" t="s">
+      <c r="E42" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F42" s="9"/>
+      <c r="F42" s="14"/>
       <c r="G42" s="3">
         <v>5</v>
       </c>
@@ -3674,10 +3680,10 @@
       <c r="I42" s="4"/>
     </row>
     <row r="43" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="9"/>
+      <c r="F43" s="14"/>
       <c r="G43" s="5">
         <v>3</v>
       </c>
@@ -3687,19 +3693,31 @@
       <c r="I43" s="4"/>
     </row>
     <row r="44" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+    </row>
+    <row r="46" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E46" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="34">
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
     <mergeCell ref="E44:F44"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
@@ -3712,9 +3730,6 @@
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="E42:F42"/>
     <mergeCell ref="E43:F43"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A10:L10"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
@@ -3723,13 +3738,14 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A10:L10"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="55" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="55" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reporte que incluye Assessment Center
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Modelo de Gestión por Competencias</t>
   </si>
@@ -73,12 +73,15 @@
   <si>
     <t>Promedio ponderado</t>
   </si>
+  <si>
+    <t>Variable equivalente</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,8 +134,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,8 +154,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -169,11 +184,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -195,25 +236,55 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -320,7 +391,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$34</c:f>
+              <c:f>Hoja1!$E$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -364,7 +435,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$E$33</c:f>
+              <c:f>Hoja1!$E$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -375,7 +446,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$34</c:f>
+              <c:f>Hoja1!$H$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -391,7 +462,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$35</c:f>
+              <c:f>Hoja1!$E$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -435,7 +506,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$E$33</c:f>
+              <c:f>Hoja1!$E$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -446,7 +517,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$35</c:f>
+              <c:f>Hoja1!$H$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -462,7 +533,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$36</c:f>
+              <c:f>Hoja1!$E$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -506,7 +577,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$E$33</c:f>
+              <c:f>Hoja1!$E$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -517,7 +588,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$36</c:f>
+              <c:f>Hoja1!$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -533,7 +604,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$37</c:f>
+              <c:f>Hoja1!$E$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -574,7 +645,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$37</c:f>
+              <c:f>Hoja1!$H$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -587,7 +658,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$38</c:f>
+              <c:f>Hoja1!$E$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -628,7 +699,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$38</c:f>
+              <c:f>Hoja1!$H$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -641,7 +712,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$39</c:f>
+              <c:f>Hoja1!$E$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -682,7 +753,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$39</c:f>
+              <c:f>Hoja1!$H$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -695,7 +766,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$40</c:f>
+              <c:f>Hoja1!$E$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -741,7 +812,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$40</c:f>
+              <c:f>Hoja1!$H$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -754,7 +825,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$41</c:f>
+              <c:f>Hoja1!$E$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -800,7 +871,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$41</c:f>
+              <c:f>Hoja1!$H$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -813,7 +884,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$42</c:f>
+              <c:f>Hoja1!$E$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -859,7 +930,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$42</c:f>
+              <c:f>Hoja1!$H$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -872,7 +943,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$43</c:f>
+              <c:f>Hoja1!$E$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -918,7 +989,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$43</c:f>
+              <c:f>Hoja1!$H$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -936,11 +1007,11 @@
         </c:dLbls>
         <c:gapWidth val="355"/>
         <c:overlap val="-70"/>
-        <c:axId val="239645224"/>
-        <c:axId val="239645616"/>
+        <c:axId val="168253088"/>
+        <c:axId val="168280944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="239645224"/>
+        <c:axId val="168253088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -983,7 +1054,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239645616"/>
+        <c:crossAx val="168280944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -991,7 +1062,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239645616"/>
+        <c:axId val="168280944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1109,7 +1180,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239645224"/>
+        <c:crossAx val="168253088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1271,7 +1342,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$H$33</c:f>
+              <c:f>Hoja1!$I$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1320,7 +1391,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$E$34:$E$43</c:f>
+              <c:f>Hoja1!$E$32:$E$41</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1337,7 +1408,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$H$34:$H$43</c:f>
+              <c:f>Hoja1!$I$32:$I$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1359,7 +1430,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$I$33</c:f>
+              <c:f>Hoja1!$J$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1408,7 +1479,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$E$34:$E$43</c:f>
+              <c:f>Hoja1!$E$32:$E$41</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1425,7 +1496,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$I$34:$I$43</c:f>
+              <c:f>Hoja1!$J$32:$J$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1441,11 +1512,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239646400"/>
-        <c:axId val="242267984"/>
+        <c:axId val="168396200"/>
+        <c:axId val="168402088"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="239646400"/>
+        <c:axId val="168396200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1488,7 +1559,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242267984"/>
+        <c:crossAx val="168402088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1496,7 +1567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242267984"/>
+        <c:axId val="168402088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1547,7 +1618,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239646400"/>
+        <c:crossAx val="168396200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2813,13 +2884,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>74082</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2842,15 +2913,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>179918</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>15345</xdr:rowOff>
+      <xdr:colOff>122768</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>186795</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1079500</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>137583</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>60325</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3135,10 +3206,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43:I43"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3146,269 +3217,276 @@
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
-    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="6" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="11"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C4" s="12" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="H4" s="12" t="s">
+      <c r="D4" s="19"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C5" s="12" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="H5" s="12" t="s">
+      <c r="D5" s="19"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="H6" s="12" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="12"/>
     </row>
-    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E33" s="9" t="s">
+    <row r="31" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E31" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="2" t="s">
+      <c r="F31" s="21"/>
+      <c r="G31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="J31" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E34" s="14" t="s">
+    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E32" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="3">
+      <c r="F32" s="23"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="3">
         <v>2</v>
       </c>
-      <c r="H34" s="4">
+      <c r="I32" s="4">
         <v>2</v>
       </c>
-      <c r="I34" s="4"/>
+      <c r="J32" s="4"/>
     </row>
-    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E35" s="14" t="s">
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E33" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="3">
+      <c r="F33" s="16"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="3">
         <v>2</v>
       </c>
-      <c r="H35" s="4">
+      <c r="I33" s="4">
         <v>2</v>
       </c>
-      <c r="I35" s="4"/>
+      <c r="J33" s="4"/>
     </row>
-    <row r="36" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E36" s="14" t="s">
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E34" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="3">
+      <c r="F34" s="16"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="3">
         <v>3</v>
       </c>
-      <c r="H36" s="4">
+      <c r="I34" s="4">
         <v>3</v>
       </c>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="3"/>
       <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="4"/>
+    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="3"/>
       <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="4"/>
+    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="3"/>
       <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="4"/>
+    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="3"/>
       <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="4"/>
+    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="5"/>
       <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="4"/>
+    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="7"/>
       <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
+    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
     </row>
-    <row r="43" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-    </row>
-    <row r="44" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-    </row>
-    <row r="46" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E46" s="9" t="s">
+    <row r="44" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E44" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="9"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="28">
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G44:H44"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="55" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificaciones requeridas en los reportes
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
@@ -77,14 +77,14 @@
     <t>Variable equivalente</t>
   </si>
   <si>
-    <t>hola</t>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,18 +143,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -176,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -214,16 +202,9 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
+      <right style="thin">
         <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -277,6 +258,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -300,26 +292,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -331,22 +323,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -361,42 +381,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -421,7 +412,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -432,8 +423,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -453,7 +442,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -466,8 +455,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -481,13 +468,13 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="8"/>
+        <sz val="9"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -500,52 +487,16 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -559,6 +510,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -631,11 +589,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -644,8 +602,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="es-MX"/>
-              <a:t>Análisis de cobertura de Requisitos</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Valoración Relativa</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -664,11 +622,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -683,11 +641,12 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:radarChart>
-        <c:radarStyle val="filled"/>
-        <c:varyColors val="0"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -695,29 +654,181 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Candidato Ideal</c:v>
+                  <c:v>Valor Relativo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:alpha val="10196"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln w="50800">
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFC000"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$E$32:$E$42</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Capacitación Formal</c:v>
                 </c:pt>
@@ -726,9 +837,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Experiencia</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>hola</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -752,65 +860,6 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja1!$I$31</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Calificación</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4">
-                <a:alpha val="10196"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln w="50800">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Hoja1!$E$32:$E$42</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Capacitación Formal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Capacitación Complementaria</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Experiencia</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>hola</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$I$32:$I$42</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -819,11 +868,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="164938232"/>
-        <c:axId val="164938624"/>
-      </c:radarChart>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="164623192"/>
+        <c:axId val="164623576"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="164938232"/>
+        <c:axId val="164623192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,7 +888,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="dk1">
+              <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -853,9 +904,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -866,7 +917,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164938624"/>
+        <c:crossAx val="164623576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -874,7 +925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164938624"/>
+        <c:axId val="164623576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -884,7 +935,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
+                <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -894,6 +945,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CR"/>
+                  <a:t>Ponderación</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -912,9 +1019,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -925,7 +1032,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164938232"/>
+        <c:crossAx val="164623192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -937,62 +1044,17 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="100000">
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="43000">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="dk1">
+        <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1034,6 +1096,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CR"/>
+              <a:t>Análisis de Cobertura de Requisitos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1067,31 +1154,81 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:radarChart>
+        <c:radarStyle val="marker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$I$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Candidato Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$E$32:$E$42</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Capacitación Formal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Capacitación Complementaria</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Experiencia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$32</c:f>
+              <c:f>Hoja1!$I$32:$I$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1100,100 +1237,76 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$J$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Calificación</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$E$32:$E$42</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Capacitación Formal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Capacitación Complementaria</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Experiencia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$33</c:f>
+              <c:f>Hoja1!$J$32:$J$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$G$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$G$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$G$36</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1206,48 +1319,16 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="206203784"/>
-        <c:axId val="206204176"/>
-      </c:barChart>
+        <c:axId val="164614616"/>
+        <c:axId val="164489440"/>
+      </c:radarChart>
       <c:catAx>
-        <c:axId val="206203784"/>
+        <c:axId val="164614616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-CR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1285,7 +1366,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206204176"/>
+        <c:crossAx val="164489440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1293,7 +1374,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206204176"/>
+        <c:axId val="164489440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1313,39 +1394,8 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-CR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1375,7 +1425,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206203784"/>
+        <c:crossAx val="164614616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1388,7 +1438,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1537,547 +1587,6 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="319">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="43000">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="10196"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="50800">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="30000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="10196"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="50800">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="30000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="50800" cap="rnd" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="30000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="0" kern="1200" spc="70" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="0"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="63500" cap="rnd" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2580,24 +2089,529 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>122768</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>186795</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>60325</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1390650</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>118533</xdr:rowOff>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Gráfico 8"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2614,20 +2628,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447676</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2646,10 +2660,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="E31:I35" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
-  <autoFilter ref="E31:I35"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="E31:J42" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="E31:J42"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Méritos y Habilidades" dataDxfId="3"/>
+    <tableColumn id="2" name="Column1"/>
     <tableColumn id="3" name="Variable equivalente"/>
     <tableColumn id="4" name="Valor Relativo" dataDxfId="2"/>
     <tableColumn id="5" name="Candidato Ideal" dataDxfId="1"/>
@@ -2922,10 +2937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32:J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2933,246 +2948,302 @@
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
-    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="6" max="6" width="0.140625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="10"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="11"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="8"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C4" s="21" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="21" t="s">
+      <c r="D4" s="30"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="1"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C5" s="21" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="21" t="s">
+      <c r="D5" s="30"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="1"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="21" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="1"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="11"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="8"/>
     </row>
-    <row r="31" spans="5:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="E31" s="28" t="s">
+    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E31" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="29" t="s">
+      <c r="F31" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G31" s="30" t="s">
+      <c r="H31" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="30" t="s">
+      <c r="I31" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="31" t="s">
+      <c r="J31" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E32" s="22" t="s">
+    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E32" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="13">
+      <c r="F32" s="4"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="2">
         <v>2</v>
       </c>
-      <c r="H32" s="3">
+      <c r="I32" s="2">
         <v>2</v>
       </c>
-      <c r="I32" s="23"/>
+      <c r="J32" s="12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E33" s="22" t="s">
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E33" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="13">
+      <c r="F33" s="4"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="2">
         <v>2</v>
       </c>
-      <c r="H33" s="3">
+      <c r="I33" s="2">
         <v>2</v>
       </c>
-      <c r="I33" s="23"/>
+      <c r="J33" s="12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E34" s="16" t="s">
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E34" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="25"/>
-      <c r="G34" s="24">
+      <c r="F34" s="4"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="18">
         <v>3</v>
       </c>
-      <c r="H34" s="26">
+      <c r="I34" s="18">
         <v>3</v>
       </c>
-      <c r="I34" s="27"/>
+      <c r="J34" s="19">
+        <v>1</v>
+      </c>
     </row>
-    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E35" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" s="25"/>
-      <c r="G35" s="33">
-        <v>5</v>
-      </c>
-      <c r="H35" s="34"/>
-      <c r="I35" s="35"/>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E35" s="10"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2">
+        <v>4</v>
+      </c>
+      <c r="J35" s="12">
+        <v>2</v>
+      </c>
     </row>
-    <row r="36" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E36" s="13"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
+    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E36" s="10"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2">
+        <v>3</v>
+      </c>
+      <c r="J36" s="12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E37" s="13"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
+    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E37" s="10"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2">
+        <v>2</v>
+      </c>
+      <c r="J37" s="12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="38" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E38" s="13"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
+    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E38" s="17"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2">
+        <v>2</v>
+      </c>
+      <c r="J38" s="12">
+        <v>2</v>
+      </c>
     </row>
-    <row r="39" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="13"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
+    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E39" s="17"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18">
+        <v>3</v>
+      </c>
+      <c r="J39" s="19">
+        <v>3</v>
+      </c>
     </row>
-    <row r="40" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E40" s="13"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
+    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E40" s="17"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="19"/>
     </row>
-    <row r="41" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="13"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="6"/>
+    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E41" s="26"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="23"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E42" s="16"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
+    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E42" s="26"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
     </row>
-    <row r="44" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E44" s="15" t="s">
+    <row r="43" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E44" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="9"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A8:K8"/>
+  <mergeCells count="17">
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A8:L8"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F44:G44"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="55" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Grafico de barras igual al de araña
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
@@ -305,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -370,6 +370,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -383,6 +386,9 @@
     </xf>
     <xf numFmtId="2" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -602,9 +608,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Valoración Relativa</a:t>
+              <a:rPr lang="es-CR" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Análisis de Cobertura de Requisitos</a:t>
             </a:r>
+            <a:endParaRPr lang="es-CR" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -617,26 +628,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -650,180 +641,25 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$H$31</c:f>
+              <c:f>Hoja1!$I$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Valor Relativo</c:v>
+                  <c:v>Candidato Ideal</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="10"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$E$32:$E$42</c:f>
@@ -843,7 +679,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$H$32:$H$42</c:f>
+              <c:f>Hoja1!$I$32:$I$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -854,6 +690,96 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$J$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Calificación</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$E$32:$E$42</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Capacitación Formal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Capacitación Complementaria</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Experiencia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$J$32:$J$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -870,11 +796,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="164623192"/>
-        <c:axId val="164623576"/>
+        <c:axId val="165010440"/>
+        <c:axId val="164682120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="164623192"/>
+        <c:axId val="165010440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -917,7 +843,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164623576"/>
+        <c:crossAx val="164682120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -925,7 +851,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164623576"/>
+        <c:axId val="164682120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -980,26 +906,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-CR"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1032,7 +938,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164623192"/>
+        <c:crossAx val="165010440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1044,6 +950,11 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1319,11 +1230,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="164614616"/>
-        <c:axId val="164489440"/>
+        <c:axId val="188751080"/>
+        <c:axId val="188751464"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="164614616"/>
+        <c:axId val="188751080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1366,7 +1277,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164489440"/>
+        <c:crossAx val="188751464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1374,7 +1285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164489440"/>
+        <c:axId val="188751464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1425,7 +1336,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164614616"/>
+        <c:crossAx val="188751080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1546,550 +1457,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2939,8 +2307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32:J42"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2960,100 +2328,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
       <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
       <c r="M2" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="30"/>
+      <c r="I5" s="31"/>
       <c r="J5" s="27"/>
       <c r="K5" s="27"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
       <c r="L6" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
       <c r="M8" s="8"/>
     </row>
     <row r="31" spans="5:10" x14ac:dyDescent="0.25">
@@ -3217,12 +2585,12 @@
       <c r="J43" s="3"/>
     </row>
     <row r="44" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E44" s="33" t="s">
+      <c r="E44" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="F44" s="33"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="31"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
       <c r="I44" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Valores exactos en el grafico Aporte de EC y AC
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
@@ -369,6 +369,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -383,18 +395,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -662,7 +662,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$E$32:$E$42</c:f>
+              <c:f>Hoja1!$E$32:$E$41</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -679,10 +679,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$I$32:$I$42</c:f>
+              <c:f>Hoja1!$I$32:$I$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -737,7 +737,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$E$32:$E$42</c:f>
+              <c:f>Hoja1!$E$32:$E$41</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -754,10 +754,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$J$32:$J$42</c:f>
+              <c:f>Hoja1!$J$32:$J$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -796,11 +796,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="165010440"/>
-        <c:axId val="164682120"/>
+        <c:axId val="264610608"/>
+        <c:axId val="288226528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="165010440"/>
+        <c:axId val="264610608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,7 +843,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164682120"/>
+        <c:crossAx val="288226528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -851,7 +851,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164682120"/>
+        <c:axId val="288226528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,7 +938,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165010440"/>
+        <c:crossAx val="264610608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1096,7 +1096,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$E$32:$E$42</c:f>
+              <c:f>Hoja1!$E$32:$E$41</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1113,10 +1113,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$I$32:$I$42</c:f>
+              <c:f>Hoja1!$I$32:$I$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1173,7 +1173,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$E$32:$E$42</c:f>
+              <c:f>Hoja1!$E$32:$E$41</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1190,10 +1190,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$J$32:$J$42</c:f>
+              <c:f>Hoja1!$J$32:$J$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1230,11 +1230,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188751080"/>
-        <c:axId val="188751464"/>
+        <c:axId val="288227312"/>
+        <c:axId val="288227704"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="188751080"/>
+        <c:axId val="288227312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1277,7 +1277,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188751464"/>
+        <c:crossAx val="288227704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1285,7 +1285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="188751464"/>
+        <c:axId val="288227704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1336,7 +1336,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188751080"/>
+        <c:crossAx val="288227312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2028,8 +2028,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="E31:J42" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="E31:J42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="E31:J41" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="E31:J41"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Méritos y Habilidades" dataDxfId="3"/>
     <tableColumn id="2" name="Column1"/>
@@ -2307,8 +2307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:K5"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2328,100 +2328,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
       <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
       <c r="M2" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="31"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="31"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
       <c r="L6" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
       <c r="M8" s="8"/>
     </row>
     <row r="31" spans="5:10" x14ac:dyDescent="0.25">
@@ -2585,21 +2585,16 @@
       <c r="J43" s="3"/>
     </row>
     <row r="44" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E44" s="35" t="s">
+      <c r="E44" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F44" s="35"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
       <c r="I44" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E44:F44"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:L1"/>
@@ -2612,6 +2607,11 @@
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="C6:D6"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E44:F44"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="55" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificación de la tabla en los reportes
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Modelo de Gestión por Competencias</t>
   </si>
@@ -74,17 +74,20 @@
     <t>Promedio ponderado</t>
   </si>
   <si>
-    <t>Variable equivalente</t>
+    <t>Método seleccionado</t>
   </si>
   <si>
-    <t>Column1</t>
+    <t>Varible equivalente (VE)</t>
+  </si>
+  <si>
+    <t>Calificación VE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +146,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -164,7 +174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -215,50 +225,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -292,20 +258,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -314,78 +271,53 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -393,14 +325,70 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -496,7 +484,37 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -519,46 +537,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -641,7 +619,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$I$31</c:f>
+              <c:f>Hoja1!$H$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -662,7 +640,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$E$32:$E$41</c:f>
+              <c:f>Hoja1!$C$32:$C$41</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -679,7 +657,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$I$32:$I$41</c:f>
+              <c:f>Hoja1!$H$32:$H$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -716,7 +694,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$J$31</c:f>
+              <c:f>Hoja1!$I$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -737,7 +715,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$E$32:$E$41</c:f>
+              <c:f>Hoja1!$C$32:$C$41</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -754,7 +732,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$J$32:$J$41</c:f>
+              <c:f>Hoja1!$I$32:$I$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -796,11 +774,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="264610608"/>
-        <c:axId val="288226528"/>
+        <c:axId val="157185168"/>
+        <c:axId val="158141984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="264610608"/>
+        <c:axId val="157185168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,7 +821,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288226528"/>
+        <c:crossAx val="158141984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -851,7 +829,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288226528"/>
+        <c:axId val="158141984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,7 +916,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="264610608"/>
+        <c:crossAx val="157185168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1073,7 +1051,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$I$31</c:f>
+              <c:f>Hoja1!$H$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1096,7 +1074,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$E$32:$E$41</c:f>
+              <c:f>Hoja1!$C$32:$C$41</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1113,7 +1091,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$I$32:$I$41</c:f>
+              <c:f>Hoja1!$H$32:$H$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1150,7 +1128,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$J$31</c:f>
+              <c:f>Hoja1!$I$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1173,7 +1151,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$E$32:$E$41</c:f>
+              <c:f>Hoja1!$C$32:$C$41</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1190,7 +1168,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$J$32:$J$41</c:f>
+              <c:f>Hoja1!$I$32:$I$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1230,11 +1208,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="288227312"/>
-        <c:axId val="288227704"/>
+        <c:axId val="112294440"/>
+        <c:axId val="158215944"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="288227312"/>
+        <c:axId val="112294440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1277,7 +1255,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288227704"/>
+        <c:crossAx val="158215944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1285,7 +1263,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288227704"/>
+        <c:axId val="158215944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1336,7 +1314,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288227312"/>
+        <c:crossAx val="112294440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1969,13 +1947,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>14288</xdr:rowOff>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1390650</xdr:colOff>
+      <xdr:colOff>1266825</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1996,16 +1974,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>447676</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2028,15 +2006,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="E31:J41" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="E31:J41"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Méritos y Habilidades" dataDxfId="3"/>
-    <tableColumn id="2" name="Column1"/>
-    <tableColumn id="3" name="Variable equivalente"/>
-    <tableColumn id="4" name="Valor Relativo" dataDxfId="2"/>
-    <tableColumn id="5" name="Candidato Ideal" dataDxfId="1"/>
-    <tableColumn id="6" name="Calificación" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C31:I41" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="C31:I41"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Méritos y Habilidades" dataDxfId="6"/>
+    <tableColumn id="2" name="Varible equivalente (VE)"/>
+    <tableColumn id="3" name="Método seleccionado"/>
+    <tableColumn id="7" name="Calificación VE" dataDxfId="5"/>
+    <tableColumn id="4" name="Valor Relativo" dataDxfId="4"/>
+    <tableColumn id="5" name="Candidato Ideal" dataDxfId="3"/>
+    <tableColumn id="6" name="Calificación" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2305,313 +2284,339 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="0.140625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" customWidth="1"/>
-    <col min="14" max="14" width="20" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="7"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="8"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C4" s="35" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="35" t="s">
+      <c r="D4" s="23"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="35"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="1"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C5" s="35" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="35" t="s">
+      <c r="D5" s="23"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="35"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="1"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="35" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="35"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="1"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="8"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
     </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E31" s="13" t="s">
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="21" t="s">
+      <c r="D31" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="E31" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="15" t="s">
+      <c r="F31" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="I31" s="15" t="s">
+      <c r="H31" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="J31" s="16" t="s">
+      <c r="I31" s="30" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E32" s="11" t="s">
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F32" s="4"/>
-      <c r="G32" s="9"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2">
+        <v>2</v>
+      </c>
       <c r="H32" s="2">
         <v>2</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2">
         <v>2</v>
       </c>
-      <c r="J32" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E33" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="9"/>
       <c r="H33" s="2">
         <v>2</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C34" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="8">
+        <v>3</v>
+      </c>
+      <c r="H34" s="8">
+        <v>3</v>
+      </c>
+      <c r="I34" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C35" s="14"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2">
+        <v>4</v>
+      </c>
+      <c r="I35" s="7">
         <v>2</v>
       </c>
-      <c r="J33" s="12">
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C36" s="14"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2">
         <v>3</v>
       </c>
+      <c r="I36" s="7">
+        <v>3</v>
+      </c>
     </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E34" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="18">
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C37" s="14"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2">
+        <v>2</v>
+      </c>
+      <c r="I37" s="7">
         <v>3</v>
       </c>
-      <c r="I34" s="18">
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C38" s="14"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2">
+        <v>2</v>
+      </c>
+      <c r="I38" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C39" s="14"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8">
         <v>3</v>
       </c>
-      <c r="J34" s="19">
-        <v>1</v>
+      <c r="I39" s="9">
+        <v>3</v>
       </c>
     </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E35" s="10"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2">
-        <v>4</v>
-      </c>
-      <c r="J35" s="12">
-        <v>2</v>
-      </c>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C40" s="17"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="9"/>
     </row>
-    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E36" s="10"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2">
-        <v>3</v>
-      </c>
-      <c r="J36" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E37" s="10"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2">
-        <v>2</v>
-      </c>
-      <c r="J37" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E38" s="17"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2">
-        <v>2</v>
-      </c>
-      <c r="J38" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E39" s="17"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18">
-        <v>3</v>
-      </c>
-      <c r="J39" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E40" s="17"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="19"/>
-    </row>
-    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E41" s="26"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="23"/>
+    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C41" s="11"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E42" s="26"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="3"/>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="11"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="3"/>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
       <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
     </row>
-    <row r="44" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E44" s="30" t="s">
+    <row r="44" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E44" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F44" s="30"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="6"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="29">
+        <v>2.5875498499999998</v>
+      </c>
+      <c r="H44" s="29"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="A8:L8"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="55" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificación de reportes, nuevas templates
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Modelo de Gestión por Competencias</t>
   </si>
@@ -82,12 +82,18 @@
   <si>
     <t>Calificación VE</t>
   </si>
+  <si>
+    <t>Firma Evaluador</t>
+  </si>
+  <si>
+    <t>Firma Colaborador</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +159,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -174,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -218,19 +232,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -258,11 +259,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -277,10 +296,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -290,9 +309,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -300,24 +316,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -325,70 +347,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -539,6 +514,52 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -619,7 +640,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$H$31</c:f>
+              <c:f>Hoja1!$G$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -640,7 +661,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$C$32:$C$41</c:f>
+              <c:f>Hoja1!$B$35:$B$43</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -657,10 +678,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$H$32:$H$41</c:f>
+              <c:f>Hoja1!$G$35:$G$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -694,7 +715,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$I$31</c:f>
+              <c:f>Hoja1!$H$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -715,7 +736,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$C$32:$C$41</c:f>
+              <c:f>Hoja1!$B$35:$B$43</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -732,10 +753,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$I$32:$I$41</c:f>
+              <c:f>Hoja1!$H$35:$H$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -774,11 +795,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="157185168"/>
-        <c:axId val="158141984"/>
+        <c:axId val="164373952"/>
+        <c:axId val="164374344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="157185168"/>
+        <c:axId val="164373952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -821,7 +842,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="158141984"/>
+        <c:crossAx val="164374344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -829,7 +850,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158141984"/>
+        <c:axId val="164374344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -916,7 +937,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157185168"/>
+        <c:crossAx val="164373952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1051,7 +1072,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$H$31</c:f>
+              <c:f>Hoja1!$G$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1074,7 +1095,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$C$32:$C$41</c:f>
+              <c:f>Hoja1!$B$35:$B$43</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1091,10 +1112,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$H$32:$H$41</c:f>
+              <c:f>Hoja1!$G$35:$G$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1128,7 +1149,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$I$31</c:f>
+              <c:f>Hoja1!$H$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1151,7 +1172,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$C$32:$C$41</c:f>
+              <c:f>Hoja1!$B$35:$B$43</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1168,10 +1189,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$I$32:$I$41</c:f>
+              <c:f>Hoja1!$H$35:$H$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1208,11 +1229,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="112294440"/>
-        <c:axId val="158215944"/>
+        <c:axId val="164375128"/>
+        <c:axId val="164375520"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="112294440"/>
+        <c:axId val="164375128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1255,7 +1276,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="158215944"/>
+        <c:crossAx val="164375520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1263,7 +1284,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158215944"/>
+        <c:axId val="164375520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1314,7 +1335,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112294440"/>
+        <c:crossAx val="164375128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1945,15 +1966,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>57149</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1266825</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1390649</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1974,16 +1995,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1066800</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2006,16 +2027,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C31:I41" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="C31:I41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B34:H43" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="B34:H43"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Méritos y Habilidades" dataDxfId="6"/>
+    <tableColumn id="1" name="Méritos y Habilidades" dataDxfId="4"/>
     <tableColumn id="2" name="Varible equivalente (VE)"/>
     <tableColumn id="3" name="Método seleccionado"/>
-    <tableColumn id="7" name="Calificación VE" dataDxfId="5"/>
-    <tableColumn id="4" name="Valor Relativo" dataDxfId="4"/>
-    <tableColumn id="5" name="Candidato Ideal" dataDxfId="3"/>
-    <tableColumn id="6" name="Calificación" dataDxfId="2"/>
+    <tableColumn id="7" name="Calificación VE" dataDxfId="3"/>
+    <tableColumn id="4" name="Valor Relativo" dataDxfId="2"/>
+    <tableColumn id="5" name="Candidato Ideal" dataDxfId="1"/>
+    <tableColumn id="6" name="Calificación" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2284,339 +2305,370 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
       <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
       <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C4" s="23" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="23" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="1"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C5" s="23" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="23" t="s">
+      <c r="C5" s="30"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="1"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="23" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="1"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="1"/>
     </row>
-    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
     </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="19" t="s">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="C34" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="D34" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="E34" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G31" s="30" t="s">
+      <c r="F34" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="30" t="s">
+      <c r="G34" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="30" t="s">
+      <c r="H34" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="14" t="s">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2">
-        <v>2</v>
-      </c>
-      <c r="H32" s="2">
-        <v>2</v>
-      </c>
-      <c r="I32" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C33" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2">
-        <v>2</v>
-      </c>
-      <c r="H33" s="2">
-        <v>2</v>
-      </c>
-      <c r="I33" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C34" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="8">
-        <v>3</v>
-      </c>
-      <c r="H34" s="8">
-        <v>3</v>
-      </c>
-      <c r="I34" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C35" s="14"/>
+      <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2">
-        <v>4</v>
-      </c>
-      <c r="I35" s="7">
+      <c r="F35" s="2">
         <v>2</v>
       </c>
+      <c r="G35" s="2">
+        <v>2</v>
+      </c>
+      <c r="H35" s="7">
+        <v>3</v>
+      </c>
     </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C36" s="14"/>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2">
+      <c r="F36" s="2">
+        <v>2</v>
+      </c>
+      <c r="G36" s="2">
+        <v>2</v>
+      </c>
+      <c r="H36" s="7">
         <v>3</v>
       </c>
-      <c r="I36" s="7">
-        <v>3</v>
-      </c>
     </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C37" s="14"/>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2">
-        <v>2</v>
-      </c>
-      <c r="I37" s="7">
+      <c r="F37" s="8">
         <v>3</v>
       </c>
+      <c r="G37" s="8">
+        <v>3</v>
+      </c>
+      <c r="H37" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C38" s="14"/>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="13"/>
+      <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2">
+      <c r="G38" s="2">
+        <v>4</v>
+      </c>
+      <c r="H38" s="7">
         <v>2</v>
       </c>
-      <c r="I38" s="7">
-        <v>2</v>
-      </c>
     </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C39" s="14"/>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="13"/>
+      <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8">
+      <c r="G39" s="2">
         <v>3</v>
       </c>
-      <c r="I39" s="9">
+      <c r="H39" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C40" s="17"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="9"/>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="13"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2">
+        <v>2</v>
+      </c>
+      <c r="H40" s="7">
+        <v>3</v>
+      </c>
     </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C41" s="11"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="13"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2">
+        <v>2</v>
+      </c>
+      <c r="H41" s="7">
+        <v>2</v>
+      </c>
     </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="13"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8">
+        <v>3</v>
+      </c>
+      <c r="H42" s="9">
+        <v>3</v>
+      </c>
     </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="16"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="9"/>
     </row>
-    <row r="44" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E44" s="21" t="s">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="11"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="11"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="11"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="4:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D49" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F44" s="22"/>
-      <c r="G44" s="29">
+      <c r="E49" s="29">
         <v>2.5875498499999998</v>
       </c>
-      <c r="H44" s="29"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="4"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="69" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="26"/>
+      <c r="H69" s="26"/>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C70" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D70" s="25"/>
+      <c r="F70" s="23" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
+  <mergeCells count="18">
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A8:L8"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="55" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificación de templates de reportes, se agregan 2 nuevas templates
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
@@ -332,6 +332,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -354,9 +357,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -795,11 +795,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="164373952"/>
-        <c:axId val="164374344"/>
+        <c:axId val="185534496"/>
+        <c:axId val="185805456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="164373952"/>
+        <c:axId val="185534496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,7 +842,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164374344"/>
+        <c:crossAx val="185805456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -850,7 +850,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164374344"/>
+        <c:axId val="185805456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,7 +937,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164373952"/>
+        <c:crossAx val="185534496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1229,11 +1229,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="164375128"/>
-        <c:axId val="164375520"/>
+        <c:axId val="186072672"/>
+        <c:axId val="185662680"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="164375128"/>
+        <c:axId val="186072672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1276,7 +1276,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164375520"/>
+        <c:crossAx val="185662680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1284,7 +1284,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164375520"/>
+        <c:axId val="185662680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1335,7 +1335,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164375128"/>
+        <c:crossAx val="186072672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2305,10 +2305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2329,100 +2329,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="30" t="s">
+      <c r="C4" s="31"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
       <c r="J4" s="15"/>
       <c r="K4" s="14"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="30" t="s">
+      <c r="C5" s="31"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="15"/>
       <c r="K6" s="14"/>
       <c r="L6" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -2621,41 +2621,36 @@
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="4:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D49" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="29">
+      <c r="E49" s="30">
         <v>2.5875498499999998</v>
       </c>
-      <c r="F49" s="29"/>
+      <c r="F49" s="30"/>
       <c r="G49" s="21"/>
       <c r="H49" s="19"/>
       <c r="I49" s="4"/>
     </row>
-    <row r="69" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="F69" s="26"/>
-      <c r="G69" s="26"/>
-      <c r="H69" s="26"/>
+    <row r="60" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="27"/>
     </row>
-    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C70" s="25" t="s">
+    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C61" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D70" s="25"/>
-      <c r="F70" s="23" t="s">
+      <c r="D61" s="26"/>
+      <c r="F61" s="23" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="F69:H69"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="E49:F49"/>
@@ -2669,6 +2664,11 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="F60:H60"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="55" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificación de templates de reportes
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluacionPorCompetenciasTemplate.xlsx
@@ -287,24 +287,12 @@
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -322,14 +310,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -338,11 +319,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -362,11 +358,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
     <dxf>
       <font>
         <b val="0"/>
@@ -378,7 +380,41 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="9"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -408,7 +444,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="9"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -440,7 +476,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="9"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -478,7 +514,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -487,11 +523,47 @@
           <color indexed="64"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -518,49 +590,23 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -621,7 +667,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -798,11 +843,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="166139040"/>
-        <c:axId val="166139432"/>
+        <c:axId val="158824696"/>
+        <c:axId val="158825088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="166139040"/>
+        <c:axId val="158824696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -845,7 +890,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166139432"/>
+        <c:crossAx val="158825088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -853,7 +898,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166139432"/>
+        <c:axId val="158825088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -899,7 +944,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -940,7 +984,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166139040"/>
+        <c:crossAx val="158824696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -954,7 +998,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1034,7 +1077,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1232,11 +1274,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166140216"/>
-        <c:axId val="166140608"/>
+        <c:axId val="158825872"/>
+        <c:axId val="158826264"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="166140216"/>
+        <c:axId val="158825872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1279,7 +1321,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166140608"/>
+        <c:crossAx val="158826264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1287,7 +1329,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166140608"/>
+        <c:axId val="158826264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1338,7 +1380,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166140216"/>
+        <c:crossAx val="158825872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1352,7 +1394,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2030,16 +2071,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B34:H43" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B34:H43" totalsRowShown="0" headerRowDxfId="0" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B34:H43"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Méritos y Habilidades" dataDxfId="4"/>
-    <tableColumn id="2" name="Varible equivalente (VE)"/>
-    <tableColumn id="3" name="Método seleccionado"/>
-    <tableColumn id="7" name="Calificación VE" dataDxfId="3"/>
-    <tableColumn id="4" name="Valor Relativo" dataDxfId="2"/>
-    <tableColumn id="5" name="Candidato Ideal" dataDxfId="1"/>
-    <tableColumn id="6" name="Calificación" dataDxfId="0"/>
+    <tableColumn id="1" name="Méritos y Habilidades" dataDxfId="7"/>
+    <tableColumn id="2" name="Varible equivalente (VE)" dataDxfId="6"/>
+    <tableColumn id="3" name="Método seleccionado" dataDxfId="5"/>
+    <tableColumn id="7" name="Calificación VE" dataDxfId="4"/>
+    <tableColumn id="4" name="Valor Relativo" dataDxfId="3"/>
+    <tableColumn id="5" name="Candidato Ideal" dataDxfId="2"/>
+    <tableColumn id="6" name="Calificación" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2310,15 +2351,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:H6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" customWidth="1"/>
@@ -2332,332 +2373,330 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="25" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="14"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="10"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="25" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="14"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="10"/>
       <c r="L6" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G34" s="20" t="s">
+      <c r="G34" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="20" t="s">
+      <c r="H34" s="32" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2">
+      <c r="C35" s="9"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18">
         <v>2</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="18">
         <v>2</v>
       </c>
-      <c r="H35" s="7">
+      <c r="H35" s="19">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2">
+      <c r="C36" s="9"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18">
         <v>2</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="18">
         <v>2</v>
       </c>
-      <c r="H36" s="7">
+      <c r="H36" s="19">
         <v>3</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="8">
+      <c r="C37" s="9"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="20">
         <v>3</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G37" s="20">
         <v>3</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="13"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2">
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18">
         <v>4</v>
       </c>
-      <c r="H38" s="7">
+      <c r="H38" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="13"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2">
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18">
         <v>3</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H39" s="19">
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="13"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2">
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18">
         <v>2</v>
       </c>
-      <c r="H40" s="7">
+      <c r="H40" s="19">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="13"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2">
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18">
         <v>2</v>
       </c>
-      <c r="H41" s="7">
+      <c r="H41" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="13"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8">
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20">
         <v>3</v>
       </c>
-      <c r="H42" s="9">
+      <c r="H42" s="21">
         <v>3</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="16"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="9"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="21"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="11"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="11"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="11"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
     </row>
     <row r="49" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D49" s="22" t="s">
+      <c r="D49" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="31">
+      <c r="E49" s="29">
         <v>2.5875498499999998</v>
       </c>
-      <c r="F49" s="31"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="19"/>
-      <c r="I49" s="4"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="3"/>
     </row>
     <row r="60" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="28"/>
-      <c r="H60" s="28"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
     </row>
     <row r="61" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C61" s="27" t="s">
+      <c r="C61" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D61" s="27"/>
-      <c r="F61" s="23" t="s">
+      <c r="D61" s="25"/>
+      <c r="F61" s="16" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="F60:H60"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="E49:F49"/>
@@ -2674,6 +2713,8 @@
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="F60:H60"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="55" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>